<commit_message>
Version 0.1 of User-Input Excel file for Aircraft input generation
Version 0.2 of Coding Guidelines

Version 0.1 of Aircraft.py
</commit_message>
<xml_diff>
--- a/userinput.xlsx
+++ b/userinput.xlsx
@@ -5,27 +5,27 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KILKISZenbook\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KILKISZenbook\Documents\Python\KBE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9F92C6-0C56-443D-8D69-6321D48B4319}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA096057-F140-45CE-B1DD-5C91B0EEEB81}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Formatted File" sheetId="1" r:id="rId1"/>
+    <sheet name="Inputs" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="2" r:id="rId2"/>
-    <sheet name="Output" sheetId="3" r:id="rId3"/>
+    <sheet name="export_ready_inputs" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ColumnTitle1">'Formatted File'!$B$4</definedName>
-    <definedName name="InputArea">'Formatted File'!$B$5:$G$10</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Formatted File'!$4:$4</definedName>
-    <definedName name="RowTitleRegion1..C2">'Formatted File'!$B$2</definedName>
-    <definedName name="RowTitleRegion2..C4">'Formatted File'!#REF!</definedName>
-    <definedName name="RowTitleRegion3..E4">'Formatted File'!#REF!</definedName>
-    <definedName name="Vehicle_1_Name">IF(RIGHT('Formatted File'!#REF!,5)="Total", TRIM(LEFT('Formatted File'!#REF!,SEARCH("TOTAL",'Formatted File'!#REF!)-1)),'Formatted File'!#REF!)</definedName>
-    <definedName name="Vehicle_2_Name">IF(RIGHT('Formatted File'!$B$3,5)="Total", TRIM(LEFT('Formatted File'!$B$3,SEARCH("TOTAL",'Formatted File'!$B$3)-1)),'Formatted File'!$B$3)</definedName>
+    <definedName name="ColumnTitle1">Inputs!$B$4</definedName>
+    <definedName name="InputArea">Inputs!$B$5:$E$10</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Inputs!$4:$4</definedName>
+    <definedName name="RowTitleRegion1..C2">Inputs!$B$2</definedName>
+    <definedName name="RowTitleRegion2..C4">Inputs!#REF!</definedName>
+    <definedName name="RowTitleRegion3..E4">Inputs!#REF!</definedName>
+    <definedName name="Vehicle_1_Name">IF(RIGHT(Inputs!#REF!,5)="Total", TRIM(LEFT(Inputs!#REF!,SEARCH("TOTAL",Inputs!#REF!)-1)),Inputs!#REF!)</definedName>
+    <definedName name="Vehicle_2_Name">IF(RIGHT(Inputs!$B$3,5)="Total", TRIM(LEFT(Inputs!$B$3,SEARCH("TOTAL",Inputs!$B$3)-1)),Inputs!$B$3)</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>UAV Design Input File</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Payload Size</t>
-  </si>
-  <si>
     <t>Hand-Launchable</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>Desired Range expressed in Kilometers</t>
   </si>
   <si>
-    <t>[m]</t>
-  </si>
-  <si>
     <t>Boolean</t>
   </si>
   <si>
@@ -166,9 +160,6 @@
     <t>Desired Payload Weight (Mass) expressed in Kilograms</t>
   </si>
   <si>
-    <t>payload_size</t>
-  </si>
-  <si>
     <t>configuration</t>
   </si>
   <si>
@@ -176,6 +167,27 @@
   </si>
   <si>
     <t>portable</t>
+  </si>
+  <si>
+    <t>Payload Type</t>
+  </si>
+  <si>
+    <t>Payload Options</t>
+  </si>
+  <si>
+    <t>EO/IR Camera</t>
+  </si>
+  <si>
+    <t>Synthetic Aperature Radar</t>
+  </si>
+  <si>
+    <t>payload_type</t>
+  </si>
+  <si>
+    <t>eoir</t>
+  </si>
+  <si>
+    <t>sar</t>
   </si>
 </sst>
 </file>
@@ -185,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3"/>
@@ -229,14 +241,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="3"/>
-      <name val="HGMaruGothicMPRO"/>
-      <family val="2"/>
-      <charset val="128"/>
     </font>
     <font>
       <b/>
@@ -392,7 +396,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -400,9 +404,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="5">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="8">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -410,7 +411,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -423,49 +423,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -521,13 +521,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>2166110</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>16565</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>17809</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -779,185 +779,147 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G11"/>
+  <dimension ref="B1:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="88.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="88.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="39" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="2:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="5"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="2:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="12" t="s">
+      <c r="D4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="22">
         <v>1</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="9" t="str">
+      <c r="D5" s="7" t="str">
         <f>IF(B5="Endurance","[h]","[km]")</f>
         <v>[h]</v>
       </c>
-      <c r="G5" s="9" t="str">
-        <f>IF(B5=Options!C2,Options!H2,Options!H3)</f>
+      <c r="E5" s="7" t="str">
+        <f>IF(B5=Options!C2,Options!J2,Options!J3)</f>
         <v>Desired Endurance expressed in Hours</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="18">
+    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="23">
         <v>0.25</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="17" t="str">
-        <f>IF(B6=Options!E2,Options!H3,Options!H4)</f>
+      <c r="D6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="12" t="str">
+        <f>IF(B6=Options!E2,Options!J3,Options!J4)</f>
         <v>Desired Range expressed in Kilometers</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="17" t="s">
+      <c r="C9" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
-        <v>11</v>
       </c>
       <c r="C10" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19" t="s">
+      <c r="D10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
+    </row>
+    <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-  </mergeCells>
-  <dataValidations xWindow="258" yWindow="333" count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:E7" xr:uid="{57F1A5B8-1640-460F-9583-A6786CDF123A}">
-      <formula1>0</formula1>
-      <formula2>0.5</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="87" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -967,7 +929,13 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="258" yWindow="333" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="258" yWindow="333" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{57F1A5B8-1640-460F-9583-A6786CDF123A}">
+          <x14:formula1>
+            <xm:f>Options!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C7</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{71BC174E-0564-4645-9BC1-A86F452C0ED6}">
           <x14:formula1>
             <xm:f>Options!$C$2:$C$3</xm:f>
@@ -982,9 +950,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FA691A5-8663-41A4-BFBA-EC0FAA1107A9}">
           <x14:formula1>
-            <xm:f>Options!$G$2:$G$3</xm:f>
+            <xm:f>Options!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C9:E10</xm:sqref>
+          <xm:sqref>C9:C10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{296B8092-F3D5-43BB-B0FF-E3E12613CCC8}">
           <x14:formula1>
@@ -1000,135 +968,155 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587AF12F-E22C-49AF-B91A-32B9F55651C7}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="22" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="20.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" style="18" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="15" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="21" t="s">
+      <c r="D3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="21" t="s">
+      <c r="F3" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="22" t="s">
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K11" s="23"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M11" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1139,70 +1127,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00611EDB-69E9-45D7-ACBF-9FAFDB386819}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="str">
-        <f>IF('Formatted File'!B5=Options!C3,Options!D2,Options!D3)</f>
+      <c r="A1" s="8" t="str">
+        <f>IF(Inputs!B5=Options!C3,Options!D2,Options!D3)</f>
         <v>range</v>
       </c>
-      <c r="B1" s="26">
-        <f>'Formatted File'!C5</f>
+      <c r="B1" s="19">
+        <f>Inputs!C5</f>
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="str">
-        <f>IF('Formatted File'!B6=Options!E2,Options!F2,Options!F3)</f>
+      <c r="A2" s="8" t="str">
+        <f>IF(Inputs!B6=Options!E2,Options!F2,Options!F3)</f>
         <v>payload</v>
       </c>
-      <c r="B2" s="26">
-        <f>'Formatted File'!C6</f>
+      <c r="B2" s="19">
+        <f>Inputs!C6</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="19" t="str">
+        <f>INDEX(Options!H2:H3, MATCH(Inputs!C7, Options!G2:G3))</f>
+        <v>eoir</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="8" t="str">
+        <f>INDEX(Options!B:B, MATCH(Inputs!C8, Options!A:A,0))</f>
+        <v>conventional</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="8" t="str">
+        <f>IF(Inputs!C9=Options!I2, "True", "False")</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="26" t="str">
-        <f>'Formatted File'!C7 &amp; ", " &amp; 'Formatted File'!D7 &amp; ", " &amp; 'Formatted File'!E7</f>
-        <v>0.1, 0.1, 0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="10" t="str">
-        <f>INDEX(Options!B:B, MATCH('Formatted File'!C8, Options!A:A,0))</f>
-        <v>conventional</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="10" t="str">
-        <f>IF('Formatted File'!C9=Options!G2, "True", "False")</f>
-        <v>True</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="10" t="str">
-        <f>IF('Formatted File'!C10=Options!G2, "True", "False")</f>
+      <c r="B6" s="8" t="str">
+        <f>IF(Inputs!C10=Options!I2, "True", "False")</f>
         <v>True</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Version 0.2 of User-Input Excel file for Aircraft input generation
Version 0.2 of Aircraft.py
</commit_message>
<xml_diff>
--- a/userinput.xlsx
+++ b/userinput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KILKISZenbook\Documents\Python\KBE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA096057-F140-45CE-B1DD-5C91B0EEEB81}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF96E15-D879-43FD-9219-B60C556B0D5C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>UAV Design Input File</t>
   </si>
@@ -188,6 +188,18 @@
   </si>
   <si>
     <t>sar</t>
+  </si>
+  <si>
+    <t>performance_goal</t>
+  </si>
+  <si>
+    <t>weight_target</t>
+  </si>
+  <si>
+    <t>goal_value</t>
+  </si>
+  <si>
+    <t>target_value</t>
   </si>
 </sst>
 </file>
@@ -450,9 +462,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -466,6 +475,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -781,8 +793,8 @@
   </sheetPr>
   <dimension ref="B1:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -819,7 +831,7 @@
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -833,8 +845,8 @@
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="22">
-        <v>1</v>
+      <c r="C5" s="21">
+        <v>10</v>
       </c>
       <c r="D5" s="7" t="str">
         <f>IF(B5="Endurance","[h]","[km]")</f>
@@ -849,7 +861,7 @@
       <c r="B6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="22">
         <v>0.25</v>
       </c>
       <c r="D6" s="12" t="s">
@@ -865,7 +877,7 @@
         <v>43</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>11</v>
@@ -878,8 +890,8 @@
       <c r="B8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>15</v>
+      <c r="C8" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>11</v>
@@ -892,7 +904,7 @@
       <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="24" t="b">
+      <c r="C9" s="23" t="b">
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -906,7 +918,7 @@
       <c r="B10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="20" t="b">
+      <c r="C10" s="19" t="b">
         <v>1</v>
       </c>
       <c r="D10" s="13" t="s">
@@ -971,7 +983,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,71 +1137,87 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00611EDB-69E9-45D7-ACBF-9FAFDB386819}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="24" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="str">
-        <f>IF(Inputs!B5=Options!C3,Options!D2,Options!D3)</f>
-        <v>range</v>
-      </c>
-      <c r="B1" s="19">
+      <c r="A1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="24" t="str">
+        <f>IF(Inputs!B5=Options!C2,Options!D2,Options!D3)</f>
+        <v>endurance</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="24">
         <f>Inputs!C5</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="24" t="str">
         <f>IF(Inputs!B6=Options!E2,Options!F2,Options!F3)</f>
         <v>payload</v>
       </c>
-      <c r="B2" s="19">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="24">
         <f>Inputs!C6</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="19" t="str">
-        <f>INDEX(Options!H2:H3, MATCH(Inputs!C7, Options!G2:G3))</f>
-        <v>eoir</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="8" t="str">
-        <f>INDEX(Options!B:B, MATCH(Inputs!C8, Options!A:A,0))</f>
-        <v>conventional</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="24" t="str">
+        <f>INDEX(Options!H2:H3, MATCH(Inputs!C7, Options!G2:G3))</f>
+        <v>sar</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="24" t="str">
+        <f>INDEX(Options!B:B, MATCH(Inputs!C8, Options!A:A,0))</f>
+        <v>twinboom</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="8" t="str">
+      <c r="B7" s="24" t="str">
         <f>IF(Inputs!C9=Options!I2, "True", "False")</f>
         <v>True</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="8" t="str">
+      <c r="B8" s="24" t="str">
         <f>IF(Inputs!C10=Options!I2, "True", "False")</f>
         <v>True</v>
       </c>

</xml_diff>

<commit_message>
Version 0.3a of Aircraft.py
Version 0.2a of WingThrustLoading.py
</commit_message>
<xml_diff>
--- a/userinput.xlsx
+++ b/userinput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KILKISZenbook\Documents\Python\KBE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF96E15-D879-43FD-9219-B60C556B0D5C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C0324A-E5DF-4405-91F1-F02E90181750}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -794,7 +794,7 @@
   <dimension ref="B1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -862,7 +862,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="22">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>13</v>
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B4" s="24">
         <f>Inputs!C6</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>